<commit_message>
Removed the scripts' reliance on the "RR_POD_MAX_MAF" spreadsheet
</commit_message>
<xml_diff>
--- a/Demand/InputData/Expected_Demand_Units_QAQC_Measurement_Values.xlsx
+++ b/Demand/InputData/Expected_Demand_Units_QAQC_Measurement_Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprashar\Documents\Github\DWRAT_DataScraping\Demand\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10B9DF5-A496-4B03-8B32-35C7304CC0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0B17BA-CE5E-47EB-BEE7-8386B6CABB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A297D415-07B9-4C85-9CA4-1CDE38BCAE7E}"/>
   </bookViews>
@@ -199,14 +199,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -525,7 +523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D74595C-3C80-49F1-9743-437EE37EBB20}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -704,47 +704,47 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <f>820569.4/325851</f>
         <v>2.5182350215282447</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4">
         <f>188444/325851</f>
         <v>0.57831340091023198</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <f>306870.6/325851</f>
         <v>0.9417512912343371</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4">
         <f>745399.4/325851</f>
         <v>2.28754676217044</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4">
         <f>949531.5/325851</f>
         <v>2.9140051741440107</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4">
         <f>34716.6/325851</f>
         <v>0.10654133330878222</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4">
         <f>3437.16/325851</f>
         <v>1.0548256718561551E-2</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4">
         <v>0</v>
       </c>
     </row>
@@ -764,40 +764,40 @@
       <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4">
-        <v>0</v>
-      </c>
-      <c r="P5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <f>3437.16/325851</f>
         <v>1.0548256718561551E-2</v>
       </c>
@@ -818,44 +818,44 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <f>312575.3/325851</f>
         <v>0.95925837269181313</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6">
         <f>285472.2/325851</f>
         <v>0.87608201294456678</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6">
         <f>137489.5/325851</f>
         <v>0.421939782293134</v>
       </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="4">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <f>36/325851</f>
         <v>1.1047994328696244E-4</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6">
         <f>86.6/325851</f>
         <v>2.6576564135141517E-4</v>
       </c>
@@ -876,7 +876,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8454921-0774-4A5A-8073-A67DDB7F796C}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>